<commit_message>
feat: add gacha currency support
</commit_message>
<xml_diff>
--- a/files/GameDB.xlsx
+++ b/files/GameDB.xlsx
@@ -1,41 +1,133 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\clairkim\clair_gamedashboard\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33238707-87C1-4BDB-8BF5-6B478F5C05EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1068" yWindow="1476" windowWidth="8688" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GameDB" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GameDB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>Playtime</t>
+  </si>
+  <si>
+    <t>StopPlay</t>
+  </si>
+  <si>
+    <t>UID</t>
+  </si>
+  <si>
+    <t>CouponURL</t>
+  </si>
+  <si>
+    <t>림버스 컴퍼니</t>
+  </si>
+  <si>
+    <t>X237321555</t>
+  </si>
+  <si>
+    <t>소녀전선2 망명</t>
+  </si>
+  <si>
+    <t>119615</t>
+  </si>
+  <si>
+    <t>명일방주</t>
+  </si>
+  <si>
+    <t>클레어#4859</t>
+  </si>
+  <si>
+    <t>https://arknights.kr/gift</t>
+  </si>
+  <si>
+    <t>브라운더스트 2</t>
+  </si>
+  <si>
+    <t>22013436</t>
+  </si>
+  <si>
+    <t>https://thebd2pulse.com</t>
+  </si>
+  <si>
+    <t>스텔라 소라</t>
+  </si>
+  <si>
+    <t>500355117</t>
+  </si>
+  <si>
+    <t>https://stellasora.kr/gift</t>
+  </si>
+  <si>
+    <t>니케</t>
+  </si>
+  <si>
+    <t>11368230</t>
+  </si>
+  <si>
+    <t>던파 모바일</t>
+  </si>
+  <si>
+    <t>헤이즈 리버브</t>
+  </si>
+  <si>
+    <t>100033547</t>
+  </si>
+  <si>
+    <t>엘든링</t>
+  </si>
+  <si>
+    <t>Gacha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
       <name val="맑은 고딕"/>
+      <family val="2"/>
       <charset val="129"/>
-      <family val="2"/>
-      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,91 +143,32 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -455,212 +488,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col width="10.8984375" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="10.8984375" customWidth="1" style="2" min="3" max="3"/>
+    <col min="3" max="3" width="10.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="B1" s="0" t="inlineStr">
-        <is>
-          <t>StartDate</t>
-        </is>
-      </c>
-      <c r="C1" s="0" t="inlineStr">
-        <is>
-          <t>EndDate</t>
-        </is>
-      </c>
-      <c r="D1" s="0" t="inlineStr">
-        <is>
-          <t>Playtime</t>
-        </is>
-      </c>
-      <c r="E1" s="0" t="inlineStr">
-        <is>
-          <t>StopPlay</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>UID</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>CouponURL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="inlineStr">
-        <is>
-          <t>림버스 컴퍼니</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>130</v>
+      </c>
+      <c r="C2" s="1">
         <v>45668</v>
       </c>
-      <c r="C2" s="1" t="n"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>X237321555</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="inlineStr">
-        <is>
-          <t>소녀전선2 망명</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="D2" s="1"/>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>150</v>
+      </c>
+      <c r="C3" s="1">
         <v>45631</v>
       </c>
-      <c r="C3" s="1" t="n"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>119615</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>명일방주</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
+      <c r="D3" s="1"/>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>600</v>
+      </c>
+      <c r="C4" s="1">
         <v>45869</v>
       </c>
-      <c r="C4" s="1" t="n"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>클레어#4859</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://arknights.kr/gift</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>브라운더스트 2</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n">
+      <c r="D4" s="1"/>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1">
         <v>45891</v>
       </c>
-      <c r="C5" s="1" t="n"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>22013436</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://thebd2pulse.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>스텔라 소라</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
+      <c r="D5" s="1"/>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6" s="1">
         <v>45950</v>
       </c>
-      <c r="C6" s="1" t="n"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>500355117</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://stellasora.kr/gift</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="inlineStr">
-        <is>
-          <t>니케</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="n">
+      <c r="D6" s="1"/>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>300</v>
+      </c>
+      <c r="C7" s="1">
         <v>45521</v>
       </c>
-      <c r="C7" s="1" t="n"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>11368230</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="inlineStr">
-        <is>
-          <t>던파 모바일</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="n">
+      <c r="D7" s="1"/>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
         <v>45254</v>
       </c>
-      <c r="C8" s="1" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="inlineStr">
-        <is>
-          <t>헤이즈 리버브</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="n">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+      <c r="C9" s="1">
         <v>45984</v>
       </c>
-      <c r="C9" s="1" t="n"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>100033547</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="inlineStr">
-        <is>
-          <t>엘든링</t>
-        </is>
-      </c>
-      <c r="B10" s="1" t="n">
+      <c r="D9" s="1"/>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
         <v>44876</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="D10" s="1">
         <v>45607</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>